<commit_message>
Logger writes to file & some bugs fixed
</commit_message>
<xml_diff>
--- a/Defects.xlsx
+++ b/Defects.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="96" windowWidth="22980" windowHeight="10056"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="22980" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>BugId</t>
   </si>
@@ -40,13 +40,31 @@
   </si>
   <si>
     <t>Fixed by</t>
+  </si>
+  <si>
+    <t>Create new discussion by SUPER USER is currently not supported. Thus, all tests regarding to discussion might fail (most of then creates discussions by SUPER USER)</t>
+  </si>
+  <si>
+    <t>MemberTests (maybe more)</t>
+  </si>
+  <si>
+    <t>Asa</t>
+  </si>
+  <si>
+    <t>Add moderator: in SubForum-&gt;addModerator-&gt;db.Entry fails.</t>
+  </si>
+  <si>
+    <t>DB (I guess)</t>
+  </si>
+  <si>
+    <t>EditDiscussion: in Discussion-&gt;editDiscussion-&gt;db.Entry fails.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,6 +195,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -193,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -267,7 +291,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -302,7 +325,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -478,46 +500,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -526,6 +548,48 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -534,24 +598,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>